<commit_message>
Adding bike lock location so I do not forget
</commit_message>
<xml_diff>
--- a/equipmentlab/labEquipmentInventory.xlsx
+++ b/equipmentlab/labEquipmentInventory.xlsx
@@ -1,18 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizzie/Documents/git/lab/labgit/equipmentlab/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{311EBD97-E3B9-E747-B828-B11BE9EB9E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Lab" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Cage" sheetId="2" r:id="rId5"/>
+    <sheet name="Lab" sheetId="1" r:id="rId1"/>
+    <sheet name="Cage" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="413">
   <si>
     <t>Location Type</t>
   </si>
@@ -1242,31 +1263,56 @@
   </si>
   <si>
     <t>BearVault</t>
+  </si>
+  <si>
+    <t>Lizzie's office: the one with old papers</t>
+  </si>
+  <si>
+    <t>bike lock</t>
+  </si>
+  <si>
+    <t>other bike lock still on bike in Lizzie's office</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m-d"/>
+    <numFmt numFmtId="164" formatCode="m\-d"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1275,46 +1321,47 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1504,24 +1551,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E290"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A267" workbookViewId="0">
+      <selection activeCell="E290" sqref="E290"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="2" width="26.25"/>
-    <col customWidth="1" min="3" max="3" width="15.75"/>
+    <col min="1" max="2" width="26.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1590,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -1553,7 +1605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -1564,10 +1616,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1578,10 +1630,10 @@
         <v>9</v>
       </c>
       <c r="D4" s="2">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1592,10 +1644,10 @@
         <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1606,10 +1658,10 @@
         <v>11</v>
       </c>
       <c r="D6" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1620,13 +1672,13 @@
         <v>12</v>
       </c>
       <c r="D7" s="2">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -1637,10 +1689,10 @@
         <v>15</v>
       </c>
       <c r="D8" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -1651,10 +1703,10 @@
         <v>16</v>
       </c>
       <c r="D9" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -1665,10 +1717,10 @@
         <v>17</v>
       </c>
       <c r="D10" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -1679,10 +1731,10 @@
         <v>18</v>
       </c>
       <c r="D11" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -1693,10 +1745,10 @@
         <v>19</v>
       </c>
       <c r="D12" s="2">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -1707,10 +1759,10 @@
         <v>20</v>
       </c>
       <c r="D13" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -1721,10 +1773,10 @@
         <v>21</v>
       </c>
       <c r="D14" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -1735,10 +1787,10 @@
         <v>22</v>
       </c>
       <c r="D15" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -1749,10 +1801,10 @@
         <v>23</v>
       </c>
       <c r="D16" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="2" t="s">
         <v>5</v>
       </c>
@@ -1763,10 +1815,10 @@
         <v>24</v>
       </c>
       <c r="D17" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
         <v>5</v>
       </c>
@@ -1777,10 +1829,10 @@
         <v>25</v>
       </c>
       <c r="D18" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
@@ -1791,13 +1843,13 @@
         <v>26</v>
       </c>
       <c r="D19" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1808,10 +1860,10 @@
         <v>28</v>
       </c>
       <c r="D20" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1822,10 +1874,10 @@
         <v>29</v>
       </c>
       <c r="D21" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1836,10 +1888,10 @@
         <v>30</v>
       </c>
       <c r="D22" s="2">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -1850,10 +1902,10 @@
         <v>31</v>
       </c>
       <c r="D23" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -1864,13 +1916,13 @@
         <v>32</v>
       </c>
       <c r="D24" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -1881,10 +1933,10 @@
         <v>34</v>
       </c>
       <c r="D25" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -1898,7 +1950,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="2" t="s">
         <v>5</v>
       </c>
@@ -1909,10 +1961,10 @@
         <v>38</v>
       </c>
       <c r="D27" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
@@ -1923,13 +1975,13 @@
         <v>39</v>
       </c>
       <c r="D28" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="2" t="s">
         <v>5</v>
       </c>
@@ -1940,10 +1992,10 @@
         <v>40</v>
       </c>
       <c r="D29" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="2" t="s">
         <v>5</v>
       </c>
@@ -1957,7 +2009,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="2" t="s">
         <v>5</v>
       </c>
@@ -1968,10 +2020,10 @@
         <v>43</v>
       </c>
       <c r="D31" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="2" t="s">
         <v>5</v>
       </c>
@@ -1982,10 +2034,10 @@
         <v>44</v>
       </c>
       <c r="D32" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="2" t="s">
         <v>5</v>
       </c>
@@ -1996,10 +2048,10 @@
         <v>45</v>
       </c>
       <c r="D33" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="2" t="s">
         <v>5</v>
       </c>
@@ -2010,10 +2062,10 @@
         <v>46</v>
       </c>
       <c r="D34" s="2">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="2" t="s">
         <v>5</v>
       </c>
@@ -2024,10 +2076,10 @@
         <v>47</v>
       </c>
       <c r="D35" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="2" t="s">
         <v>5</v>
       </c>
@@ -2038,10 +2090,10 @@
         <v>48</v>
       </c>
       <c r="D36" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="2" t="s">
         <v>5</v>
       </c>
@@ -2055,7 +2107,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="2" t="s">
         <v>5</v>
       </c>
@@ -2066,10 +2118,10 @@
         <v>51</v>
       </c>
       <c r="D38" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="2" t="s">
         <v>5</v>
       </c>
@@ -2080,10 +2132,10 @@
         <v>53</v>
       </c>
       <c r="D39" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2094,13 +2146,13 @@
         <v>54</v>
       </c>
       <c r="D40" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="2" t="s">
         <v>5</v>
       </c>
@@ -2114,7 +2166,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="2" t="s">
         <v>5</v>
       </c>
@@ -2131,7 +2183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="2" t="s">
         <v>5</v>
       </c>
@@ -2148,7 +2200,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="2" t="s">
         <v>5</v>
       </c>
@@ -2162,7 +2214,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="2" t="s">
         <v>5</v>
       </c>
@@ -2173,24 +2225,24 @@
         <v>67</v>
       </c>
       <c r="D45" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="3">
-        <v>45361.0</v>
+        <v>45361</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="2" t="s">
         <v>5</v>
       </c>
@@ -2204,7 +2256,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="2" t="s">
         <v>5</v>
       </c>
@@ -2218,7 +2270,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
@@ -2229,10 +2281,10 @@
         <v>73</v>
       </c>
       <c r="D49" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="2" t="s">
         <v>5</v>
       </c>
@@ -2243,10 +2295,10 @@
         <v>74</v>
       </c>
       <c r="D50" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="2" t="s">
         <v>5</v>
       </c>
@@ -2260,7 +2312,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="2" t="s">
         <v>5</v>
       </c>
@@ -2271,10 +2323,10 @@
         <v>78</v>
       </c>
       <c r="D52" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="2" t="s">
         <v>5</v>
       </c>
@@ -2285,29 +2337,29 @@
         <v>78</v>
       </c>
       <c r="D53" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="3">
-        <v>45420.0</v>
+        <v>45420</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D54" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B55" s="3">
-        <v>45421.0</v>
+        <v>45421</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>81</v>
@@ -2316,7 +2368,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="2" t="s">
         <v>5</v>
       </c>
@@ -2330,7 +2382,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="2" t="s">
         <v>5</v>
       </c>
@@ -2344,7 +2396,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="2" t="s">
         <v>5</v>
       </c>
@@ -2355,10 +2407,10 @@
         <v>88</v>
       </c>
       <c r="D58" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="2" t="s">
         <v>5</v>
       </c>
@@ -2369,10 +2421,10 @@
         <v>89</v>
       </c>
       <c r="D59" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="2" t="s">
         <v>5</v>
       </c>
@@ -2386,7 +2438,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="2" t="s">
         <v>5</v>
       </c>
@@ -2403,7 +2455,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="2" t="s">
         <v>5</v>
       </c>
@@ -2414,10 +2466,10 @@
         <v>95</v>
       </c>
       <c r="D62" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="2" t="s">
         <v>5</v>
       </c>
@@ -2428,10 +2480,10 @@
         <v>96</v>
       </c>
       <c r="D63" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="2" t="s">
         <v>5</v>
       </c>
@@ -2442,10 +2494,10 @@
         <v>97</v>
       </c>
       <c r="D64" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="2" t="s">
         <v>5</v>
       </c>
@@ -2456,10 +2508,10 @@
         <v>99</v>
       </c>
       <c r="D65" s="2">
-        <v>270.0</v>
-      </c>
-    </row>
-    <row r="66">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="2" t="s">
         <v>5</v>
       </c>
@@ -2473,7 +2525,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="2" t="s">
         <v>5</v>
       </c>
@@ -2490,7 +2542,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="2" t="s">
         <v>5</v>
       </c>
@@ -2507,26 +2559,26 @@
         <v>104</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B69" s="3">
-        <v>45414.0</v>
+        <v>45414</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>106</v>
       </c>
       <c r="D69" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B70" s="3">
-        <v>45415.0</v>
+        <v>45415</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>107</v>
@@ -2535,7 +2587,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="2" t="s">
         <v>5</v>
       </c>
@@ -2549,7 +2601,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="2" t="s">
         <v>5</v>
       </c>
@@ -2563,7 +2615,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="2" t="s">
         <v>5</v>
       </c>
@@ -2574,10 +2626,10 @@
         <v>113</v>
       </c>
       <c r="D73" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="74">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="2" t="s">
         <v>5</v>
       </c>
@@ -2591,7 +2643,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="2" t="s">
         <v>5</v>
       </c>
@@ -2605,7 +2657,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76">
+    <row r="76" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="2" t="s">
         <v>5</v>
       </c>
@@ -2619,7 +2671,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="2" t="s">
         <v>5</v>
       </c>
@@ -2630,10 +2682,10 @@
         <v>121</v>
       </c>
       <c r="D77" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="2" t="s">
         <v>5</v>
       </c>
@@ -2650,7 +2702,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="2" t="s">
         <v>5</v>
       </c>
@@ -2664,7 +2716,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="2" t="s">
         <v>5</v>
       </c>
@@ -2675,13 +2727,13 @@
         <v>128</v>
       </c>
       <c r="D80" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="2" t="s">
         <v>5</v>
       </c>
@@ -2692,10 +2744,10 @@
         <v>130</v>
       </c>
       <c r="D81" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="2" t="s">
         <v>5</v>
       </c>
@@ -2706,13 +2758,13 @@
         <v>131</v>
       </c>
       <c r="D82" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A83" s="2" t="s">
         <v>5</v>
       </c>
@@ -2726,7 +2778,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A84" s="2" t="s">
         <v>5</v>
       </c>
@@ -2740,7 +2792,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A85" s="2" t="s">
         <v>5</v>
       </c>
@@ -2754,7 +2806,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A86" s="2" t="s">
         <v>5</v>
       </c>
@@ -2765,10 +2817,10 @@
         <v>137</v>
       </c>
       <c r="D86" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A87" s="2" t="s">
         <v>5</v>
       </c>
@@ -2779,10 +2831,10 @@
         <v>138</v>
       </c>
       <c r="D87" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A88" s="2" t="s">
         <v>5</v>
       </c>
@@ -2793,10 +2845,10 @@
         <v>139</v>
       </c>
       <c r="D88" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="89">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A89" s="2" t="s">
         <v>5</v>
       </c>
@@ -2807,10 +2859,10 @@
         <v>141</v>
       </c>
       <c r="D89" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A90" s="2" t="s">
         <v>5</v>
       </c>
@@ -2821,10 +2873,10 @@
         <v>142</v>
       </c>
       <c r="D90" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A91" s="2" t="s">
         <v>5</v>
       </c>
@@ -2835,10 +2887,10 @@
         <v>140</v>
       </c>
       <c r="D91" s="2">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="92">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A92" s="2" t="s">
         <v>5</v>
       </c>
@@ -2849,10 +2901,10 @@
         <v>143</v>
       </c>
       <c r="D92" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="93">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A93" s="2" t="s">
         <v>5</v>
       </c>
@@ -2863,10 +2915,10 @@
         <v>144</v>
       </c>
       <c r="D93" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A94" s="2" t="s">
         <v>5</v>
       </c>
@@ -2877,10 +2929,10 @@
         <v>146</v>
       </c>
       <c r="D94" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="95">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A95" s="2" t="s">
         <v>5</v>
       </c>
@@ -2891,10 +2943,10 @@
         <v>147</v>
       </c>
       <c r="D95" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="96">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A96" s="2" t="s">
         <v>5</v>
       </c>
@@ -2905,10 +2957,10 @@
         <v>148</v>
       </c>
       <c r="D96" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A97" s="2" t="s">
         <v>5</v>
       </c>
@@ -2922,7 +2974,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A98" s="2" t="s">
         <v>5</v>
       </c>
@@ -2933,10 +2985,10 @@
         <v>151</v>
       </c>
       <c r="D98" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A99" s="2" t="s">
         <v>5</v>
       </c>
@@ -2947,10 +2999,10 @@
         <v>152</v>
       </c>
       <c r="D99" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A100" s="2" t="s">
         <v>5</v>
       </c>
@@ -2961,10 +3013,10 @@
         <v>153</v>
       </c>
       <c r="D100" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A101" s="2" t="s">
         <v>5</v>
       </c>
@@ -2975,13 +3027,13 @@
         <v>154</v>
       </c>
       <c r="D101" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E101" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A102" s="2" t="s">
         <v>5</v>
       </c>
@@ -2992,10 +3044,10 @@
         <v>155</v>
       </c>
       <c r="D102" s="2">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="103">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A103" s="2" t="s">
         <v>5</v>
       </c>
@@ -3009,7 +3061,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="104">
+    <row r="104" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A104" s="2" t="s">
         <v>5</v>
       </c>
@@ -3020,10 +3072,10 @@
         <v>155</v>
       </c>
       <c r="D104" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A105" s="2" t="s">
         <v>5</v>
       </c>
@@ -3037,7 +3089,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A106" s="2" t="s">
         <v>5</v>
       </c>
@@ -3051,7 +3103,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A107" s="2" t="s">
         <v>5</v>
       </c>
@@ -3062,15 +3114,15 @@
         <v>161</v>
       </c>
       <c r="D107" s="2">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="108">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A108" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B108" s="3">
-        <v>45330.0</v>
+        <v>45330</v>
       </c>
       <c r="C108" s="2" t="s">
         <v>162</v>
@@ -3079,40 +3131,40 @@
         <v>163</v>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A109" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B109" s="3">
-        <v>45330.0</v>
+        <v>45330</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>164</v>
       </c>
       <c r="D109" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A110" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B110" s="3">
-        <v>45330.0</v>
+        <v>45330</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>165</v>
       </c>
       <c r="D110" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A111" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B111" s="3">
-        <v>45330.0</v>
+        <v>45330</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>166</v>
@@ -3124,7 +3176,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A112" s="2" t="s">
         <v>5</v>
       </c>
@@ -3138,7 +3190,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A113" s="2" t="s">
         <v>5</v>
       </c>
@@ -3149,10 +3201,10 @@
         <v>170</v>
       </c>
       <c r="D113" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A114" s="2" t="s">
         <v>5</v>
       </c>
@@ -3163,13 +3215,13 @@
         <v>171</v>
       </c>
       <c r="D114" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E114" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A115" s="2" t="s">
         <v>5</v>
       </c>
@@ -3180,10 +3232,10 @@
         <v>172</v>
       </c>
       <c r="D115" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A116" s="2" t="s">
         <v>5</v>
       </c>
@@ -3194,10 +3246,10 @@
         <v>174</v>
       </c>
       <c r="D116" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A117" s="2" t="s">
         <v>5</v>
       </c>
@@ -3208,242 +3260,242 @@
         <v>175</v>
       </c>
       <c r="D117" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A118" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B118" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>176</v>
       </c>
       <c r="D118" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A119" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B119" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C119" s="2" t="s">
         <v>177</v>
       </c>
       <c r="D119" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A120" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B120" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C120" s="2" t="s">
         <v>179</v>
       </c>
       <c r="D120" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A121" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B121" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C121" s="2" t="s">
         <v>180</v>
       </c>
       <c r="D121" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A122" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B122" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C122" s="2" t="s">
         <v>181</v>
       </c>
       <c r="D122" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A123" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B123" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>182</v>
       </c>
       <c r="D123" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A124" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B124" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C124" s="2" t="s">
         <v>183</v>
       </c>
       <c r="D124" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="125">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A125" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B125" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C125" s="2" t="s">
         <v>184</v>
       </c>
       <c r="D125" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="126">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A126" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B126" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>185</v>
       </c>
       <c r="D126" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A127" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B127" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C127" s="2" t="s">
         <v>186</v>
       </c>
       <c r="D127" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A128" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B128" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>187</v>
       </c>
       <c r="D128" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A129" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B129" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C129" s="2" t="s">
         <v>188</v>
       </c>
       <c r="D129" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A130" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B130" s="3">
-        <v>45333.0</v>
+        <v>45333</v>
       </c>
       <c r="C130" s="2" t="s">
         <v>189</v>
       </c>
       <c r="D130" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A131" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B131" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C131" s="2" t="s">
         <v>190</v>
       </c>
       <c r="D131" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="132">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B132" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>191</v>
       </c>
       <c r="D132" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="133">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A133" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B133" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C133" s="2" t="s">
         <v>192</v>
       </c>
       <c r="D133" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="134">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A134" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B134" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C134" s="2" t="s">
         <v>184</v>
@@ -3452,66 +3504,66 @@
         <v>193</v>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A135" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B135" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C135" s="2" t="s">
         <v>194</v>
       </c>
       <c r="D135" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="136">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A136" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B136" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C136" s="2" t="s">
         <v>195</v>
       </c>
       <c r="D136" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A137" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B137" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C137" s="2" t="s">
         <v>196</v>
       </c>
       <c r="D137" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A138" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B138" s="3">
-        <v>45302.0</v>
+        <v>45302</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>197</v>
       </c>
       <c r="D138" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A139" s="2" t="s">
         <v>5</v>
       </c>
@@ -3522,10 +3574,10 @@
         <v>182</v>
       </c>
       <c r="D139" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A140" s="2" t="s">
         <v>5</v>
       </c>
@@ -3536,10 +3588,10 @@
         <v>200</v>
       </c>
       <c r="D140" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="141">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A141" s="2" t="s">
         <v>5</v>
       </c>
@@ -3553,7 +3605,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A142" s="2" t="s">
         <v>5</v>
       </c>
@@ -3570,7 +3622,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A143" s="2" t="s">
         <v>5</v>
       </c>
@@ -3584,7 +3636,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A144" s="2" t="s">
         <v>5</v>
       </c>
@@ -3601,7 +3653,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A145" s="2" t="s">
         <v>5</v>
       </c>
@@ -3615,7 +3667,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A146" s="2" t="s">
         <v>5</v>
       </c>
@@ -3629,7 +3681,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A147" s="2" t="s">
         <v>5</v>
       </c>
@@ -3643,7 +3695,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A148" s="2" t="s">
         <v>5</v>
       </c>
@@ -3657,7 +3709,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A149" s="2" t="s">
         <v>5</v>
       </c>
@@ -3671,7 +3723,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A150" s="2" t="s">
         <v>5</v>
       </c>
@@ -3685,7 +3737,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A151" s="2" t="s">
         <v>5</v>
       </c>
@@ -3699,7 +3751,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A152" s="2" t="s">
         <v>5</v>
       </c>
@@ -3710,10 +3762,10 @@
         <v>219</v>
       </c>
       <c r="D152" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A153" s="2" t="s">
         <v>5</v>
       </c>
@@ -3724,10 +3776,10 @@
         <v>220</v>
       </c>
       <c r="D153" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A154" s="2" t="s">
         <v>5</v>
       </c>
@@ -3738,10 +3790,10 @@
         <v>221</v>
       </c>
       <c r="D154" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A155" s="2" t="s">
         <v>5</v>
       </c>
@@ -3755,7 +3807,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A156" s="2" t="s">
         <v>5</v>
       </c>
@@ -3769,7 +3821,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A157" s="2" t="s">
         <v>5</v>
       </c>
@@ -3780,10 +3832,10 @@
         <v>226</v>
       </c>
       <c r="D157" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A158" s="2" t="s">
         <v>5</v>
       </c>
@@ -3794,13 +3846,13 @@
         <v>227</v>
       </c>
       <c r="D158" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A159" s="2" t="s">
         <v>5</v>
       </c>
@@ -3811,10 +3863,10 @@
         <v>229</v>
       </c>
       <c r="D159" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A160" s="2" t="s">
         <v>5</v>
       </c>
@@ -3831,7 +3883,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A161" s="2" t="s">
         <v>5</v>
       </c>
@@ -3845,7 +3897,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A162" s="2" t="s">
         <v>5</v>
       </c>
@@ -3859,7 +3911,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A163" s="2" t="s">
         <v>5</v>
       </c>
@@ -3870,10 +3922,10 @@
         <v>238</v>
       </c>
       <c r="D163" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A164" s="2" t="s">
         <v>5</v>
       </c>
@@ -3884,10 +3936,10 @@
         <v>239</v>
       </c>
       <c r="D164" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A165" s="2" t="s">
         <v>5</v>
       </c>
@@ -3898,10 +3950,10 @@
         <v>240</v>
       </c>
       <c r="D165" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A166" s="2" t="s">
         <v>5</v>
       </c>
@@ -3912,10 +3964,10 @@
         <v>241</v>
       </c>
       <c r="D166" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="167">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A167" s="2" t="s">
         <v>5</v>
       </c>
@@ -3926,10 +3978,10 @@
         <v>243</v>
       </c>
       <c r="D167" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A168" s="2" t="s">
         <v>5</v>
       </c>
@@ -3940,10 +3992,10 @@
         <v>244</v>
       </c>
       <c r="D168" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A169" s="2" t="s">
         <v>5</v>
       </c>
@@ -3954,10 +4006,10 @@
         <v>245</v>
       </c>
       <c r="D169" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="170">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A170" s="2" t="s">
         <v>5</v>
       </c>
@@ -3968,10 +4020,10 @@
         <v>246</v>
       </c>
       <c r="D170" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A171" s="2" t="s">
         <v>5</v>
       </c>
@@ -3982,10 +4034,10 @@
         <v>248</v>
       </c>
       <c r="D171" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A172" s="2" t="s">
         <v>5</v>
       </c>
@@ -3996,10 +4048,10 @@
         <v>249</v>
       </c>
       <c r="D172" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A173" s="2" t="s">
         <v>5</v>
       </c>
@@ -4010,10 +4062,10 @@
         <v>250</v>
       </c>
       <c r="D173" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A174" s="2" t="s">
         <v>5</v>
       </c>
@@ -4024,10 +4076,10 @@
         <v>251</v>
       </c>
       <c r="D174" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="175">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A175" s="2" t="s">
         <v>5</v>
       </c>
@@ -4038,10 +4090,10 @@
         <v>252</v>
       </c>
       <c r="D175" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A176" s="2" t="s">
         <v>5</v>
       </c>
@@ -4052,10 +4104,10 @@
         <v>197</v>
       </c>
       <c r="D176" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A177" s="2" t="s">
         <v>5</v>
       </c>
@@ -4069,7 +4121,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A178" s="2" t="s">
         <v>5</v>
       </c>
@@ -4080,10 +4132,10 @@
         <v>256</v>
       </c>
       <c r="D178" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A179" s="2" t="s">
         <v>5</v>
       </c>
@@ -4094,10 +4146,10 @@
         <v>257</v>
       </c>
       <c r="D179" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A180" s="2" t="s">
         <v>5</v>
       </c>
@@ -4108,10 +4160,10 @@
         <v>258</v>
       </c>
       <c r="D180" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A181" s="2" t="s">
         <v>5</v>
       </c>
@@ -4122,10 +4174,10 @@
         <v>259</v>
       </c>
       <c r="D181" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A182" s="2" t="s">
         <v>5</v>
       </c>
@@ -4136,10 +4188,10 @@
         <v>261</v>
       </c>
       <c r="D182" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="183">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A183" s="2" t="s">
         <v>5</v>
       </c>
@@ -4150,10 +4202,10 @@
         <v>262</v>
       </c>
       <c r="D183" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="184">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A184" s="2" t="s">
         <v>5</v>
       </c>
@@ -4167,7 +4219,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A185" s="2" t="s">
         <v>5</v>
       </c>
@@ -4178,10 +4230,10 @@
         <v>267</v>
       </c>
       <c r="D185" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A186" s="2" t="s">
         <v>5</v>
       </c>
@@ -4195,7 +4247,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A187" s="2" t="s">
         <v>5</v>
       </c>
@@ -4206,10 +4258,10 @@
         <v>269</v>
       </c>
       <c r="D187" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A188" s="2" t="s">
         <v>5</v>
       </c>
@@ -4220,10 +4272,10 @@
         <v>270</v>
       </c>
       <c r="D188" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A189" s="2" t="s">
         <v>5</v>
       </c>
@@ -4234,10 +4286,10 @@
         <v>271</v>
       </c>
       <c r="D189" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A190" s="2" t="s">
         <v>5</v>
       </c>
@@ -4248,10 +4300,10 @@
         <v>272</v>
       </c>
       <c r="D190" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A191" s="2" t="s">
         <v>5</v>
       </c>
@@ -4262,10 +4314,10 @@
         <v>273</v>
       </c>
       <c r="D191" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="192">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A192" s="2" t="s">
         <v>5</v>
       </c>
@@ -4276,10 +4328,10 @@
         <v>261</v>
       </c>
       <c r="D192" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A193" s="2" t="s">
         <v>5</v>
       </c>
@@ -4290,10 +4342,10 @@
         <v>274</v>
       </c>
       <c r="D193" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A194" s="2" t="s">
         <v>5</v>
       </c>
@@ -4304,10 +4356,10 @@
         <v>275</v>
       </c>
       <c r="D194" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A195" s="2" t="s">
         <v>5</v>
       </c>
@@ -4318,141 +4370,141 @@
         <v>276</v>
       </c>
       <c r="D195" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="196">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A196" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B196" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>277</v>
       </c>
       <c r="D196" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A197" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B197" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>278</v>
       </c>
       <c r="D197" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="198">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A198" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B198" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>279</v>
       </c>
       <c r="D198" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A199" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B199" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D199" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="200">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A200" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B200" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>280</v>
       </c>
       <c r="D200" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A201" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B201" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>131</v>
       </c>
       <c r="D201" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="202">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A202" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B202" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>281</v>
       </c>
       <c r="D202" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="203">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A203" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B203" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>282</v>
       </c>
       <c r="D203" s="2">
-        <v>200.0</v>
-      </c>
-    </row>
-    <row r="204">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A204" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B204" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>138</v>
       </c>
       <c r="D204" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A205" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B205" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>283</v>
@@ -4461,12 +4513,12 @@
         <v>284</v>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A206" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B206" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>75</v>
@@ -4475,21 +4527,21 @@
         <v>284</v>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A207" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B207" s="3">
-        <v>45383.0</v>
+        <v>45383</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>285</v>
       </c>
       <c r="D207" s="2">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="208">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A208" s="2" t="s">
         <v>5</v>
       </c>
@@ -4500,10 +4552,10 @@
         <v>287</v>
       </c>
       <c r="D208" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A209" s="2" t="s">
         <v>5</v>
       </c>
@@ -4514,10 +4566,10 @@
         <v>288</v>
       </c>
       <c r="D209" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A210" s="2" t="s">
         <v>5</v>
       </c>
@@ -4528,10 +4580,10 @@
         <v>289</v>
       </c>
       <c r="D210" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A211" s="2" t="s">
         <v>5</v>
       </c>
@@ -4542,10 +4594,10 @@
         <v>290</v>
       </c>
       <c r="D211" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="212">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A212" s="2" t="s">
         <v>5</v>
       </c>
@@ -4556,10 +4608,10 @@
         <v>291</v>
       </c>
       <c r="D212" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="213">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A213" s="2" t="s">
         <v>5</v>
       </c>
@@ -4573,7 +4625,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A214" s="2" t="s">
         <v>5</v>
       </c>
@@ -4587,7 +4639,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A215" s="2" t="s">
         <v>5</v>
       </c>
@@ -4598,10 +4650,10 @@
         <v>296</v>
       </c>
       <c r="D215" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A216" s="2" t="s">
         <v>5</v>
       </c>
@@ -4615,7 +4667,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A217" s="2" t="s">
         <v>5</v>
       </c>
@@ -4626,10 +4678,10 @@
         <v>300</v>
       </c>
       <c r="D217" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A218" s="2" t="s">
         <v>5</v>
       </c>
@@ -4640,15 +4692,15 @@
         <v>301</v>
       </c>
       <c r="D218" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="219">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A219" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B219" s="3">
-        <v>45387.0</v>
+        <v>45387</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>103</v>
@@ -4657,7 +4709,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A220" s="2" t="s">
         <v>5</v>
       </c>
@@ -4668,10 +4720,10 @@
         <v>303</v>
       </c>
       <c r="D220" s="2">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="221">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A221" s="2" t="s">
         <v>5</v>
       </c>
@@ -4682,10 +4734,10 @@
         <v>305</v>
       </c>
       <c r="D221" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="222">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A222" s="2" t="s">
         <v>5</v>
       </c>
@@ -4699,7 +4751,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A223" s="2" t="s">
         <v>5</v>
       </c>
@@ -4710,10 +4762,10 @@
         <v>307</v>
       </c>
       <c r="D223" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="224">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A224" s="2" t="s">
         <v>5</v>
       </c>
@@ -4727,7 +4779,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A225" s="2" t="s">
         <v>5</v>
       </c>
@@ -4738,10 +4790,10 @@
         <v>309</v>
       </c>
       <c r="D225" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="226">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A226" s="2" t="s">
         <v>5</v>
       </c>
@@ -4752,10 +4804,10 @@
         <v>310</v>
       </c>
       <c r="D226" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A227" s="2" t="s">
         <v>5</v>
       </c>
@@ -4766,10 +4818,10 @@
         <v>311</v>
       </c>
       <c r="D227" s="2">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="228">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A228" s="2" t="s">
         <v>5</v>
       </c>
@@ -4783,7 +4835,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A229" s="2" t="s">
         <v>5</v>
       </c>
@@ -4797,7 +4849,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A230" s="2" t="s">
         <v>5</v>
       </c>
@@ -4808,10 +4860,10 @@
         <v>317</v>
       </c>
       <c r="D230" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A231" s="2" t="s">
         <v>5</v>
       </c>
@@ -4822,10 +4874,10 @@
         <v>318</v>
       </c>
       <c r="D231" s="2">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="232">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A232" s="2" t="s">
         <v>5</v>
       </c>
@@ -4836,10 +4888,10 @@
         <v>319</v>
       </c>
       <c r="D232" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A233" s="2" t="s">
         <v>5</v>
       </c>
@@ -4850,24 +4902,24 @@
         <v>320</v>
       </c>
       <c r="D233" s="2">
-        <v>72.0</v>
-      </c>
-    </row>
-    <row r="234">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A234" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B234" s="3">
-        <v>45392.0</v>
+        <v>45392</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>303</v>
       </c>
       <c r="D234" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="235">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A235" s="2" t="s">
         <v>321</v>
       </c>
@@ -4878,10 +4930,10 @@
         <v>323</v>
       </c>
       <c r="D235" s="2">
-        <v>48.0</v>
-      </c>
-    </row>
-    <row r="236">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A236" s="2" t="s">
         <v>321</v>
       </c>
@@ -4892,10 +4944,10 @@
         <v>324</v>
       </c>
       <c r="D236" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="237">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A237" s="2" t="s">
         <v>321</v>
       </c>
@@ -4906,10 +4958,10 @@
         <v>325</v>
       </c>
       <c r="D237" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="238">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A238" s="2" t="s">
         <v>321</v>
       </c>
@@ -4923,7 +4975,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A239" s="2" t="s">
         <v>321</v>
       </c>
@@ -4937,7 +4989,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="1:4" ht="13" x14ac:dyDescent="0.15">
       <c r="A240" s="2" t="s">
         <v>321</v>
       </c>
@@ -4948,10 +5000,10 @@
         <v>330</v>
       </c>
       <c r="D240" s="2">
-        <v>500.0</v>
-      </c>
-    </row>
-    <row r="241">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A241" s="2" t="s">
         <v>321</v>
       </c>
@@ -4965,7 +5017,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="242">
+    <row r="242" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A242" s="2" t="s">
         <v>321</v>
       </c>
@@ -4979,7 +5031,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="243">
+    <row r="243" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A243" s="2" t="s">
         <v>321</v>
       </c>
@@ -4990,10 +5042,10 @@
         <v>333</v>
       </c>
       <c r="D243" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="244">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A244" s="2" t="s">
         <v>321</v>
       </c>
@@ -5004,10 +5056,10 @@
         <v>334</v>
       </c>
       <c r="D244" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="245">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A245" s="2" t="s">
         <v>321</v>
       </c>
@@ -5018,10 +5070,10 @@
         <v>335</v>
       </c>
       <c r="D245" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="246">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A246" s="2" t="s">
         <v>321</v>
       </c>
@@ -5035,7 +5087,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="247">
+    <row r="247" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A247" s="2" t="s">
         <v>321</v>
       </c>
@@ -5049,7 +5101,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="248">
+    <row r="248" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A248" s="2" t="s">
         <v>321</v>
       </c>
@@ -5060,10 +5112,10 @@
         <v>188</v>
       </c>
       <c r="D248" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A249" s="2" t="s">
         <v>321</v>
       </c>
@@ -5074,10 +5126,10 @@
         <v>340</v>
       </c>
       <c r="D249" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A250" s="2" t="s">
         <v>321</v>
       </c>
@@ -5091,7 +5143,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="251">
+    <row r="251" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A251" s="2" t="s">
         <v>321</v>
       </c>
@@ -5105,7 +5157,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="252">
+    <row r="252" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A252" s="2" t="s">
         <v>321</v>
       </c>
@@ -5116,10 +5168,10 @@
         <v>345</v>
       </c>
       <c r="D252" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A253" s="2" t="s">
         <v>321</v>
       </c>
@@ -5130,10 +5182,10 @@
         <v>346</v>
       </c>
       <c r="D253" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="254">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A254" s="2" t="s">
         <v>321</v>
       </c>
@@ -5150,7 +5202,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="255">
+    <row r="255" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A255" s="2" t="s">
         <v>321</v>
       </c>
@@ -5161,13 +5213,13 @@
         <v>349</v>
       </c>
       <c r="D255" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E255" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="256">
+    <row r="256" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A256" s="2" t="s">
         <v>321</v>
       </c>
@@ -5178,13 +5230,13 @@
         <v>350</v>
       </c>
       <c r="D256" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E256" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="257">
+    <row r="257" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A257" s="2" t="s">
         <v>321</v>
       </c>
@@ -5201,7 +5253,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="258">
+    <row r="258" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A258" s="2" t="s">
         <v>321</v>
       </c>
@@ -5212,11 +5264,11 @@
         <v>353</v>
       </c>
       <c r="D258" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E258" s="2"/>
     </row>
-    <row r="259">
+    <row r="259" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A259" s="2" t="s">
         <v>321</v>
       </c>
@@ -5227,10 +5279,10 @@
         <v>355</v>
       </c>
       <c r="D259" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A260" s="2" t="s">
         <v>321</v>
       </c>
@@ -5241,10 +5293,10 @@
         <v>356</v>
       </c>
       <c r="D260" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A261" s="2" t="s">
         <v>321</v>
       </c>
@@ -5255,13 +5307,13 @@
         <v>357</v>
       </c>
       <c r="D261" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="E261" s="2" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="262">
+    <row r="262" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A262" s="2" t="s">
         <v>321</v>
       </c>
@@ -5272,10 +5324,10 @@
         <v>359</v>
       </c>
       <c r="D262" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A263" s="2" t="s">
         <v>321</v>
       </c>
@@ -5286,13 +5338,13 @@
         <v>360</v>
       </c>
       <c r="D263" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E263" s="2" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="264">
+    <row r="264" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A264" s="2" t="s">
         <v>321</v>
       </c>
@@ -5303,10 +5355,10 @@
         <v>362</v>
       </c>
       <c r="D264" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A265" s="2" t="s">
         <v>321</v>
       </c>
@@ -5320,7 +5372,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="266">
+    <row r="266" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A266" s="2" t="s">
         <v>321</v>
       </c>
@@ -5331,10 +5383,10 @@
         <v>365</v>
       </c>
       <c r="D266" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A267" s="2" t="s">
         <v>321</v>
       </c>
@@ -5348,7 +5400,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="268">
+    <row r="268" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A268" s="2" t="s">
         <v>321</v>
       </c>
@@ -5359,10 +5411,10 @@
         <v>367</v>
       </c>
       <c r="D268" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="269">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A269" s="2" t="s">
         <v>321</v>
       </c>
@@ -5373,10 +5425,10 @@
         <v>368</v>
       </c>
       <c r="D269" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="270">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A270" s="2" t="s">
         <v>321</v>
       </c>
@@ -5387,10 +5439,10 @@
         <v>369</v>
       </c>
       <c r="D270" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A271" s="2" t="s">
         <v>321</v>
       </c>
@@ -5401,10 +5453,10 @@
         <v>370</v>
       </c>
       <c r="D271" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A272" s="2" t="s">
         <v>321</v>
       </c>
@@ -5415,10 +5467,10 @@
         <v>371</v>
       </c>
       <c r="D272" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A273" s="2" t="s">
         <v>321</v>
       </c>
@@ -5429,10 +5481,10 @@
         <v>372</v>
       </c>
       <c r="D273" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A274" s="2" t="s">
         <v>321</v>
       </c>
@@ -5443,13 +5495,13 @@
         <v>374</v>
       </c>
       <c r="D274" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="E274" s="2" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="275">
+    <row r="275" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A275" s="2" t="s">
         <v>321</v>
       </c>
@@ -5460,10 +5512,10 @@
         <v>376</v>
       </c>
       <c r="D275" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A276" s="2" t="s">
         <v>321</v>
       </c>
@@ -5474,10 +5526,10 @@
         <v>377</v>
       </c>
       <c r="D276" s="2">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="277">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A277" s="2" t="s">
         <v>321</v>
       </c>
@@ -5488,10 +5540,10 @@
         <v>356</v>
       </c>
       <c r="D277" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A278" s="2" t="s">
         <v>321</v>
       </c>
@@ -5502,10 +5554,10 @@
         <v>378</v>
       </c>
       <c r="D278" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="279">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A279" s="2" t="s">
         <v>321</v>
       </c>
@@ -5519,7 +5571,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="280">
+    <row r="280" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A280" s="2" t="s">
         <v>321</v>
       </c>
@@ -5533,7 +5585,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="281">
+    <row r="281" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A281" s="2" t="s">
         <v>321</v>
       </c>
@@ -5544,10 +5596,10 @@
         <v>382</v>
       </c>
       <c r="D281" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A282" s="2" t="s">
         <v>321</v>
       </c>
@@ -5558,13 +5610,13 @@
         <v>383</v>
       </c>
       <c r="D282" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E282" s="2" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="283">
+    <row r="283" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A283" s="2" t="s">
         <v>321</v>
       </c>
@@ -5578,7 +5630,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="284">
+    <row r="284" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A284" s="2" t="s">
         <v>321</v>
       </c>
@@ -5592,7 +5644,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="285">
+    <row r="285" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A285" s="2" t="s">
         <v>321</v>
       </c>
@@ -5603,10 +5655,10 @@
         <v>389</v>
       </c>
       <c r="D285" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A286" s="2" t="s">
         <v>321</v>
       </c>
@@ -5617,10 +5669,10 @@
         <v>390</v>
       </c>
       <c r="D286" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A287" s="2" t="s">
         <v>321</v>
       </c>
@@ -5634,7 +5686,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="288">
+    <row r="288" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A288" s="2" t="s">
         <v>321</v>
       </c>
@@ -5645,10 +5697,10 @@
         <v>393</v>
       </c>
       <c r="D288" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" ht="13" x14ac:dyDescent="0.15">
       <c r="A289" s="2" t="s">
         <v>321</v>
       </c>
@@ -5659,25 +5711,43 @@
         <v>394</v>
       </c>
       <c r="D289" s="2">
-        <v>1.0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A290" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B290" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C290" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="D290" s="5">
+        <v>1</v>
+      </c>
+      <c r="E290" s="5" t="s">
+        <v>412</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -5688,23 +5758,23 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
         <v>395</v>
       </c>
       <c r="B2" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>396</v>
       </c>
       <c r="B3" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>397</v>
       </c>
@@ -5715,77 +5785,77 @@
         <v>399</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
         <v>400</v>
       </c>
       <c r="B5" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
         <v>401</v>
       </c>
       <c r="B6" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
         <v>402</v>
       </c>
       <c r="B7" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="2" t="s">
         <v>403</v>
       </c>
       <c r="B8" s="2">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
         <v>404</v>
       </c>
       <c r="B9" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="2" t="s">
         <v>406</v>
       </c>
       <c r="B10" s="2">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="2" t="s">
         <v>407</v>
       </c>
       <c r="B11" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
         <v>409</v>
       </c>
       <c r="B12" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>